<commit_message>
Prepare for adding dc
</commit_message>
<xml_diff>
--- a/Examples/paper_port/PortCoupling_IEEE14Bus.xlsx
+++ b/Examples/paper_port/PortCoupling_IEEE14Bus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Examples\paper_port coupling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Examples\Paper_Port\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1178F252-E4A1-43AE-A58A-7233857A11C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CCAEA4-649D-4B0A-B1C1-5A7884055EA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>